<commit_message>
Latest Tableau and House Cleaning
</commit_message>
<xml_diff>
--- a/tableau/Tableau Change Log.xlsx
+++ b/tableau/Tableau Change Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teradata.sharepoint.com/teams/2019Teams-Covid19dashboard/Shared Documents/Covid19 dashboard/Tableau Samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{13708DBD-4FF2-4C1E-83B3-F648A7F9A03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{290230FC-904E-486F-89CD-B3C595D359A1}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{13708DBD-4FF2-4C1E-83B3-F648A7F9A03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57F08BFC-165C-46F4-A6E2-C4E4C95B7898}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{01455932-1564-402F-BA8D-1E5065AB49FC}"/>
   </bookViews>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>Date/Time</t>
   </si>
@@ -42,6 +43,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Who</t>
   </si>
   <si>
     <t>7/15/2020  6:23 PM CT</t>
@@ -52,6 +56,9 @@
 3 I got a new image with the name in the graphic (so it looks better "responsive to resolution" but something is weird for top header bar on first dashboard vs the others_x000D_
 4 New Dashboard Hospital rates is there _x000D_
 5 Known data issues:  TD Sites are still missing</t>
+  </si>
+  <si>
+    <t>CH</t>
   </si>
   <si>
     <t>7/15/2020  10PM CT</t>
@@ -331,6 +338,22 @@
 NEW DATA SOURCE: F_IND_DASH_GOOGLE_TRENDS_V
 3 8-28 full data refresh
 4 8-28 added google search text re: instability in API</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>10/2/2020 3PM CT</t>
+  </si>
+  <si>
+    <t>v0.20.3</t>
+  </si>
+  <si>
+    <t>1 Data sources p2 updates
+2 Hosp Rates: Added reference band to all graphs showing no data 8/13-8/27 and updated tool tips with desc of data source</t>
   </si>
 </sst>
 </file>
@@ -712,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41B9ECC-374F-4739-81FE-01203D780024}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -725,7 +748,7 @@
     <col min="3" max="3" width="117.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -735,247 +758,335 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="99.75">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="99.75">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>0.06</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>0.01</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="142.5">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="142.5">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>0.02</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="270.75">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="270.75">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>0.03</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>0.03</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.5">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>0.04</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="171">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="171">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>0.05</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="99.75">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="99.75">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>0.06</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="142.5">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="142.5">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="42.75">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="42.75">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2">
         <v>0.08</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="213.75">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="213.75">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>0.09</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="42.75">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="42.75">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="199.5">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="199.5">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="156.75">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="156.75">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="99.75">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="99.75">
       <c r="A16" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <v>0.13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="71.25">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="71.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="99.75">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="99.75">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="42.75">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="42.75">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>0.16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="42.75">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="42.75">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2">
         <v>0.17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="299.25">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="299.25">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <v>0.18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="57">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="57">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2">
         <v>0.19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="75">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="75">
       <c r="A23" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2">
         <v>0.2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30">
+      <c r="A25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -985,15 +1096,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0BB004135BA7E438DDEE5AFF9643195" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02fa29c6f17eb6796f211e3309d1ac57">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="68ec2f0f-435b-4dc7-b5ba-99cb48143b1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="775a2d29a009bf4d25d1edb95a55125d" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0BB004135BA7E438DDEE5AFF9643195" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eae2ae7ef03fbf5c5da41f15b480c523">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="68ec2f0f-435b-4dc7-b5ba-99cb48143b1e" xmlns:ns3="4a00ed4c-990f-4df9-a190-9a828495fe35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6c715e37c016a4d8210a4d06a7201f9" ns2:_="" ns3:_="">
     <xsd:import namespace="68ec2f0f-435b-4dc7-b5ba-99cb48143b1e"/>
+    <xsd:import namespace="4a00ed4c-990f-4df9-a190-9a828495fe35"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1007,6 +1122,8 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1052,6 +1169,36 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4a00ed4c-990f-4df9-a190-9a828495fe35" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1155,22 +1302,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1328D086-0485-43CB-A09D-E0EB716A1EF9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA8B386C-3C69-4B1B-B91D-4B5C526CED7C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B56EABCE-C029-4492-9CAD-52D628540395}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64FD2C3D-4839-4F20-8597-4B0CDB384BC4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA8B386C-3C69-4B1B-B91D-4B5C526CED7C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1328D086-0485-43CB-A09D-E0EB716A1EF9}"/>
 </file>
</xml_diff>